<commit_message>
Multiple Login with DataProvider, ExtentReport and ITest Listener
</commit_message>
<xml_diff>
--- a/Automation2020/src/test/resources/Excel_Data/Testdata1.xlsx
+++ b/Automation2020/src/test/resources/Excel_Data/Testdata1.xlsx
@@ -8,37 +8,40 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
-  <si>
-    <t>Sn</t>
-  </si>
-  <si>
-    <t>uname</t>
-  </si>
-  <si>
-    <t>pass</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>danish.ali@hipster-inc.com</t>
   </si>
+  <si>
+    <t>danish.ali+1@hipster-inc.com</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -58,13 +61,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -357,64 +366,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="2.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
+      <c r="B1">
         <v>123456789</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>2</v>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>123456789</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4">
+      <c r="B2">
         <v>123456789</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>